<commit_message>
upload 23 11 2020
</commit_message>
<xml_diff>
--- a/Silamoney/TestData/datafile.xlsx
+++ b/Silamoney/TestData/datafile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="879">
   <si>
     <t xml:space="preserve">privatekeys</t>
   </si>
@@ -2033,6 +2033,630 @@
   </si>
   <si>
     <t>0x1aaecd8d3f52887f20390fcdc7041ce6321b56f3</t>
+  </si>
+  <si>
+    <t>2c0ef60bc8d660217ababc6dd195db6a3d95a2bc35dbef36e1ae9f11ad2b4548</t>
+  </si>
+  <si>
+    <t>193f0337a21f9acbca7843ef5ca87be121e4de497f763936aa128766a50b45fb</t>
+  </si>
+  <si>
+    <t>d3dbdb22d72b85a859e367df0e832df252428703f1acdef1f492dfbca65253e4</t>
+  </si>
+  <si>
+    <t>ae0819b41333759bef5895fe2f6928c671d47e01dcd570293792733353435a1b</t>
+  </si>
+  <si>
+    <t>0x1617c3ecf73780d9a3f66424a304b9290334ab25</t>
+  </si>
+  <si>
+    <t>440f0f3a820f27f768d0abd4216cc8a50ba240d26769007b193e42726eb2a8ee</t>
+  </si>
+  <si>
+    <t>dad04fe70b0e7200ceb303e9b78f0e1a9aac17b2094c9555e6339a3802302468</t>
+  </si>
+  <si>
+    <t>75f17eae6fead329a8972b5a3dc9163a64768e4b3c1eeb8a666ff50abacd031d</t>
+  </si>
+  <si>
+    <t>0x3e3d7c396a93de2123c7e1445b3bd3675b52497a</t>
+  </si>
+  <si>
+    <t>12fa02764e286687460573af33e92927b1ba6688d0ba0499bb026afce123f277</t>
+  </si>
+  <si>
+    <t>bbe2b936b7f6132063187f348464a02e4d7878da55d81c06e4784438fc0946c2</t>
+  </si>
+  <si>
+    <t>b67a33ee392e057925544420351cf5b7dea6b670742cdd90d69c7c4846eb8b28</t>
+  </si>
+  <si>
+    <t>d0316906268b58b26627eced95e2a4577348a1a424704498be2999881fca5820</t>
+  </si>
+  <si>
+    <t>0xf0e2b906f2c3eb3b113ee552bbf6f97221334ec6</t>
+  </si>
+  <si>
+    <t>24610eb91081cf99dedca94ef3dc039e9217c8c3eed2c02f524b3f1bcfc86b15</t>
+  </si>
+  <si>
+    <t>9967da937f483f0b996aa568b305fd12ac9c98fbe60cc5b3f6148845d3d0adb4</t>
+  </si>
+  <si>
+    <t>6fe6dd69ef8af5dc5a38399112753ee07f8f1b9657eb2dc5fb30136cf663f839</t>
+  </si>
+  <si>
+    <t>0x0b8a1ce7c997dc9e32297624a506d93202615421</t>
+  </si>
+  <si>
+    <t>d37694c2083a3fcbd360aec30f54274694317d1c69d3d852ffc8d9b98d02a9ce</t>
+  </si>
+  <si>
+    <t>183d6820d89709d59894edcabc21330d2d1944bee03ebaa5e381173f0bd3f188</t>
+  </si>
+  <si>
+    <t>e61c2b80432c94cb42767a48382a7f59396b13bd743df548e9a273d702613158</t>
+  </si>
+  <si>
+    <t>13ec41ec2729544f585f76818474082abb7e4093ba8823d3e244d59cf66c9fd1</t>
+  </si>
+  <si>
+    <t>0x656bb9fc2af76da0be231f9c7cdbf0a46efdfe16</t>
+  </si>
+  <si>
+    <t>b7dd2d110e7411a14e5637e45ae7d7affc5f6129d65ae20f36d940e11bb2dd0b</t>
+  </si>
+  <si>
+    <t>4f39bd38664d8784fb6b743532ce36b9188cc0b783fc29a41ef37eeb663cad60</t>
+  </si>
+  <si>
+    <t>97c2dd9fdf0ae2fa37b779d93f6711963df81bc70d4d7f728b6e3d8c4b7b95a</t>
+  </si>
+  <si>
+    <t>0x3e42e3bff3c84b1826847888d062c47eaa22cc54</t>
+  </si>
+  <si>
+    <t>c8a742caf8b83476d829bea49a4569d4d9124f4086539960a30e78c23272b6e4</t>
+  </si>
+  <si>
+    <t>26b62683e540b9e222d8330c06598b29dbff94683206b41f7b1ebfbc4ed271d9</t>
+  </si>
+  <si>
+    <t>9cc9971a50799f727eaf3bd4cc6472aeb879169e0eec8b8b13d6413f3576dbea</t>
+  </si>
+  <si>
+    <t>34fd436269a1afdf81f3395ce691de65d08cc51cc889958e5a299ac5a283d038</t>
+  </si>
+  <si>
+    <t>0xe811a22dc2be09c73328ad923edab6f879f74899</t>
+  </si>
+  <si>
+    <t>ea1708fb22c4a14a9d2ed775a6d0c97c5ebc27dd69527c18bcbf008b2465fa0e</t>
+  </si>
+  <si>
+    <t>a4d4faa257c0552d8d683bf8c13546f406e34a5fbfeb7d8ed7ee1cdeed874a15</t>
+  </si>
+  <si>
+    <t>8f34a032d55baad074b313c17fb908e0ef529e6a32f5893518660cf09a1e3f96</t>
+  </si>
+  <si>
+    <t>0x00bf73fd2a4d791bf4572b83904f3b5d3f14d563</t>
+  </si>
+  <si>
+    <t>9670542cf21daf333131abae529167d9326eaf675e3c9d4438b70e6a5eacb90e</t>
+  </si>
+  <si>
+    <t>db3844ebb774d5389ad0897874a84aa46bc4c27857a75db7ff1c4eb19ed8ac9c</t>
+  </si>
+  <si>
+    <t>a8c237819721f0978c11134e763fc996382c753052abab527fe21be44f6fe66</t>
+  </si>
+  <si>
+    <t>8a6f036030060d67bf6c54802f6c01af835d406006d04e34e3272790cccf84ab</t>
+  </si>
+  <si>
+    <t>0x7e0681d83896d54e3425914155060378facad9d8</t>
+  </si>
+  <si>
+    <t>a21e18b04b1cecf4af0b87575112c63ae0079469e8c0ca1d5875f3e43cb584db</t>
+  </si>
+  <si>
+    <t>7129cbed3ce89b375087985e8e3401df49ff708364d030668de3a1b23f877136</t>
+  </si>
+  <si>
+    <t>733dfa03ac66c9122afa3bac3eb1fa8cb2b8679c2d9b5016ed870dc848acb589</t>
+  </si>
+  <si>
+    <t>0x82b52bae0c14222c3a2aa543b342deb85868beed</t>
+  </si>
+  <si>
+    <t>1db81f253aca1bda417ce876be199153a098a7c5166745220871effb7e5c4966</t>
+  </si>
+  <si>
+    <t>7d3adc52ecb779dba418804d1491ca036cffc85c5460cc08b39780fa7e2f1006</t>
+  </si>
+  <si>
+    <t>d1bc33b085ebdb686e9bedab85cb7180a3ad16ec58852d932d38032058ecb8d3</t>
+  </si>
+  <si>
+    <t>b2b54b849aad9685b23273cf0c7f1a2c95ec4a9e8574113d00824970b4f3ed7d</t>
+  </si>
+  <si>
+    <t>0x7220f3a491b46f54a37f76afd5f70fdbe725e6a9</t>
+  </si>
+  <si>
+    <t>61e86bbf4d6f487767cc311a20d70d07e1fd6bcf8efc34be02ee138e8e8a5084</t>
+  </si>
+  <si>
+    <t>29999b1cf031702d9af78cf3fd2a259d86111075b69fb40836b819cdcebe07e8</t>
+  </si>
+  <si>
+    <t>7f959197c9aaa8589252412d15eb3c9e1fb54e7fc4a67725f0f0b065032c3a9f</t>
+  </si>
+  <si>
+    <t>0xc30184d32103f5738b64406c54a51f5f8c4a1d9e</t>
+  </si>
+  <si>
+    <t>c5365332b61e4d7c52d9fdb74daf7ba800253f76f268a2f07befd584fe36e15a</t>
+  </si>
+  <si>
+    <t>8c8468ff938d9f7d555a78ed64474ccc3df60c4d34b392f2a4fca7c0dbbaac29</t>
+  </si>
+  <si>
+    <t>9e3d2493b8eb98b9ffdfccb70f1b8fa4a17e5e0a0c0259c242f1dccd43b79312</t>
+  </si>
+  <si>
+    <t>5e8d97025e615fccccd49a7b1b4c3ffd4f98859d2be8f1f1b4026975ade6af5e</t>
+  </si>
+  <si>
+    <t>0x126b5bf8c33e6240871cfe95c1e3667118c7bb90</t>
+  </si>
+  <si>
+    <t>effef7085b7b860b51f0c1f05fe362fc5085e3358b0e5ec0304282e5b977d2b4</t>
+  </si>
+  <si>
+    <t>4dd0431acef0ade3012335dc7f722c6cd6571ad099f8080240d5d104d94a6481</t>
+  </si>
+  <si>
+    <t>878227faf995d801edb88df7d4db9118a75ad5085e7ff5097d945f3ba4bfc798</t>
+  </si>
+  <si>
+    <t>0x49f7cb23c8061c4796ed427346cd19d54037fa0f</t>
+  </si>
+  <si>
+    <t>95bc501bc6038374f0adbebe5e6b61caee66528a1e00753b40cff703e0713161</t>
+  </si>
+  <si>
+    <t>132e00543606ed1ca4f366ec6815d8f22304c7750d5cd91dc00323b06a10e588</t>
+  </si>
+  <si>
+    <t>b4c346df28e1237769e12d23f40ef145c560774796be0bbe2b4e3be04168ff3b</t>
+  </si>
+  <si>
+    <t>35bf1192cb493982ab234a9737c0af9df2f92b7e7cbbc8265e0a039f08b08e48</t>
+  </si>
+  <si>
+    <t>0x8f9de8e8ea88268d3ed7b4b6ea373f0a358ce6da</t>
+  </si>
+  <si>
+    <t>bda220d73d0314d870f708b2485070b75e23c3594ed60a1420d2d0a66edb6131</t>
+  </si>
+  <si>
+    <t>ca5044431ee84c572deb31383f94cc0f56b26896338c5c45c6cbd8ecec99bce8</t>
+  </si>
+  <si>
+    <t>81ae9782cb5d61183d682c48a8a678134b8d0a211fad2c2275349d6b62675e45</t>
+  </si>
+  <si>
+    <t>7f5dc535fb446abb1d1179aaf952f447d17e4c6161aaf56a75c1137a50a0e7d4</t>
+  </si>
+  <si>
+    <t>b152c22ccf35e61da9a78086818c0e1d0f4c6020957e6f8803ecfb428b278910</t>
+  </si>
+  <si>
+    <t>9c55c2836a1bcb32c2d2eeef6997e4d3cb979b930a6ff2b53a12904c83d67771</t>
+  </si>
+  <si>
+    <t>0x20296d748fee3cc6ab113c6b92c8f6b68c7e33a7</t>
+  </si>
+  <si>
+    <t>bd0018377eb3f7b28389b11171c909bda1a8ea0f215e0dcef88f4e6321f0bbdc</t>
+  </si>
+  <si>
+    <t>bf29dc52e2a257236d6e8db6f2efca42a2f2b4844aab29415ae0f6c2d63877a5</t>
+  </si>
+  <si>
+    <t>8b9780beb45b5b6246824cbdc814905cee51f0dc748d8c692b9b8b23547b13ad</t>
+  </si>
+  <si>
+    <t>0x31b37446cafc93ace6855e795823e92c5a2c6d59</t>
+  </si>
+  <si>
+    <t>94c101d88751cd677bbc0a8f1eff7759c39402efbe7011a13f3e9ef6ae293e69</t>
+  </si>
+  <si>
+    <t>2ec35c0060e18c2591bff8b2729cade40784fef6e5c3bd5edf7244780819f3b6</t>
+  </si>
+  <si>
+    <t>cd650088cc46cab5e05c9070800ef6da69a3818635b7b2c660862a0eda517563</t>
+  </si>
+  <si>
+    <t>c5a4b8b976df78dab13561fe2b9d290df0b4f9ec125c38b46d68939be9c94d8a</t>
+  </si>
+  <si>
+    <t>0x5ecdc8dcd0bf88f57b53434025d7ec8c56c4522f</t>
+  </si>
+  <si>
+    <t>f52a41f8de6bfcd36fdddb2b18c438778978ff22fe9f3d954cdf4d507ce9d7d</t>
+  </si>
+  <si>
+    <t>1cd70566161929c7323f5aeb0db0da23ee51e69fd8f0ff05827ecfbf3f4ee34</t>
+  </si>
+  <si>
+    <t>3ebe7093e7ca7741007f5538c3905d90926e64a25b29af42d84cfcc6e5e744fa</t>
+  </si>
+  <si>
+    <t>0x33439b25fcf110541f230d96da6ffecfb4a90e36</t>
+  </si>
+  <si>
+    <t>1e9a8ec941dae764ab17592b2139022ebfd2d49906e704b05ab5c404ab796c68</t>
+  </si>
+  <si>
+    <t>0x15c629aa52fb923f5f852eba46067aedf040701f</t>
+  </si>
+  <si>
+    <t>4d613e508bf75087746c91bfa7ee5d3060483dee72c51c949b9a625c4c105571</t>
+  </si>
+  <si>
+    <t>0x8927afe286a171561a5720f3877c2bf240177707</t>
+  </si>
+  <si>
+    <t>544826d423edd900ad20d5bcd102a5c7db4b45ad0e9205488c880c480f48d14f</t>
+  </si>
+  <si>
+    <t>1dfcf3403300694d73a3376e153ff9e66ee5d4b9bf83aa8cb2bcf521dcef706e</t>
+  </si>
+  <si>
+    <t>bfd0a682c27f1d84342662ba524ddbfcb273c4a11c2d74abf918dee39c5606b9</t>
+  </si>
+  <si>
+    <t>50667e63e155138b65407a9e84013988a9014a03a47538dea5225bfd24edf1a0</t>
+  </si>
+  <si>
+    <t>0x8386472dc80d195f21f5e64eb7e84c35bac85d99</t>
+  </si>
+  <si>
+    <t>e7dc1cccb7371f5743c6c9e4a3ff3b366ac0dcd5dc8714531e613e4f5a7901f</t>
+  </si>
+  <si>
+    <t>5c9cb7968d9eb7df00f3c6727b5357ae156149e4442278caaec9264e8252ba22</t>
+  </si>
+  <si>
+    <t>34280c0e1bb2b7edfc11fc31a84151cb87b0a7c98eabff4e76657eca0e9b330e</t>
+  </si>
+  <si>
+    <t>0x37dc9cb4897f339f333a6ec0c13f67e33a25ec18</t>
+  </si>
+  <si>
+    <t>cc412bc08796ee8b42586ea1c1a2211fe354bdf067ef27388a3cc4d273127f27</t>
+  </si>
+  <si>
+    <t>eb819ade1b7a44763d85c2e30c36321480f0a3537f3428203544b5d24d9e849c</t>
+  </si>
+  <si>
+    <t>22f91a01f581c8235e70215b73150cce04792c6f305a761b5ff49078afeb95e9</t>
+  </si>
+  <si>
+    <t>e1a7608eaaa94132040423758fcb4f105f8795de70aa50494ea65b8e8f90795d</t>
+  </si>
+  <si>
+    <t>0x97463fb6b551a4a11c4e987f91042e3fc88fe4c2</t>
+  </si>
+  <si>
+    <t>546aa293c793c035eb046c6bbf37a5ae82cef06f26cd05a38fc761d9658a032c</t>
+  </si>
+  <si>
+    <t>e5c84da0731b99a6d5389529bee7271398f9ca750332545a2248c40bf9feee06</t>
+  </si>
+  <si>
+    <t>f6427791d671ce57d7e2dd0e9d9eba89dec140ff3cc041f67e9d93edf48103c5</t>
+  </si>
+  <si>
+    <t>0x099511f73383ff450cd2900ceb4b4e24d5500c1b</t>
+  </si>
+  <si>
+    <t>1553d6357b1238f9f8559c6438dc7c2c2dcb982917545127546a8b07ef0bbad</t>
+  </si>
+  <si>
+    <t>fed8db3d99c68b66f361b7b87a9c7fafc1e8427ba581a3053521650e2dbff6b</t>
+  </si>
+  <si>
+    <t>e84dfe77a3ff44148d8b2ed9547cdf028ca35458ba94bd20c6568da6867323cc</t>
+  </si>
+  <si>
+    <t>2cf89c10c3f46261699ba5cb3b22060863a99cd512e5e51fc80452dd7258f5ac</t>
+  </si>
+  <si>
+    <t>0xd38d4fedd20026c378c62faecef630a205f7cbbc</t>
+  </si>
+  <si>
+    <t>80745f041e9afd1213bde135576e8e9febe49a06f5f5ec38424d22b0ffbdf665</t>
+  </si>
+  <si>
+    <t>bcf4de508672a7cfc2be2358813b25df09b254d40b7f71779fe349f4844125c0</t>
+  </si>
+  <si>
+    <t>643f5590214031425a8eef0408c5adbf050cf0c00b52b04fee1f891d590e7036</t>
+  </si>
+  <si>
+    <t>1a8a85cca5280013a3950c2ba619a62de0fadff4393399feeb84c8d86ee7c5ca</t>
+  </si>
+  <si>
+    <t>2d81d44306bd9bf71724be95f304b2032961c5e07be72966fb7da840d25505b8</t>
+  </si>
+  <si>
+    <t>0x4e3f97b44b36cd8968993ef61ccad874d9c3c758</t>
+  </si>
+  <si>
+    <t>39a4110062eabfbd26da68bba825efa93c05c3460044633e8c1b6148a0d6db7f</t>
+  </si>
+  <si>
+    <t>f1268c2179abe04e0443cf46704385101e3060b5a6f46716939c8785a7d95a9d</t>
+  </si>
+  <si>
+    <t>a819ecc90da5873acd56c2bc191f9ff79e0b833598c22889063e07cdd8e07f7c</t>
+  </si>
+  <si>
+    <t>b26937db0dce43d993bde01508a10db15ddf7d28376825f0ce6e192b7649e5bb</t>
+  </si>
+  <si>
+    <t>990921da7009a1bbe8ef9e4b0ff1cd81c89d3be75107f39f8d3d171d55e2e8bc</t>
+  </si>
+  <si>
+    <t>a3d025d0a376b5ff7e9828aba08f33c96ac3dea4130cdf6ddcf027da268099dd</t>
+  </si>
+  <si>
+    <t>954f9e8332c21af1f302516f914377d8fc8e6da19c1e924bb2cb240fed123852</t>
+  </si>
+  <si>
+    <t>3308994f90e019d72c36f927a8f4645f391428532b0b47265083dfdd486cf07a</t>
+  </si>
+  <si>
+    <t>34ad44c437f647e2e71ff33a7597c07369b1f932a05099ebce6a92e2b825be79</t>
+  </si>
+  <si>
+    <t>64cd9795fde5843272b66ae51a48fa4a0c0108cbe0287c7cdf42c8c82b147797</t>
+  </si>
+  <si>
+    <t>46eb9ecc3773f52f78ce31e16bae678c4bc86a37c506867b9d4afb19839710b1</t>
+  </si>
+  <si>
+    <t>42de21aa61fc98c549f1f4967a354552fe7a4a2d1b10f4a11d7a86f28088708d</t>
+  </si>
+  <si>
+    <t>0x7663f555e00a6de7ee90d9b9d331ff617d4c86c9</t>
+  </si>
+  <si>
+    <t>82f7e98c0950925a7464dc659e4e6801e9e5112704247282780100b04a154579</t>
+  </si>
+  <si>
+    <t>673cc8096597ae5c51d6f0510ae839626575b2c57b2606cd2328ad4ccb917489</t>
+  </si>
+  <si>
+    <t>76c3795938095c2e20eef372176782c1ceb6c566af62aab40348494399dd01c1</t>
+  </si>
+  <si>
+    <t>0x585cbd5b9ee44841ccce7981e13842cc2a75ee14</t>
+  </si>
+  <si>
+    <t>ffc0fb57f90985794e0223910718b2b461cabe180e557caebba9aeb99c3295cd</t>
+  </si>
+  <si>
+    <t>c9740b3c9c746a4fc3e0c311571e1b087c2cf571d80afdf07f2f72cb892ae827</t>
+  </si>
+  <si>
+    <t>3efa365d46cb7d24b23d1e5ce34fae5d94f3e2b3d892c495f12a3ea47ff71a5d</t>
+  </si>
+  <si>
+    <t>12c287d9245b30030ad814c9591692b917bdc233012ab63d305000d3a78a924d</t>
+  </si>
+  <si>
+    <t>0x80dcb2a5e3e3373288c4a42227d2c7c5c72622e4</t>
+  </si>
+  <si>
+    <t>5e6c98d2eb944253d86e0652a323875656bacdb1274d5ba9f2f422b01d64f169</t>
+  </si>
+  <si>
+    <t>f8a691b7db035a462e96bdf6b13c5a5fdd2e10c6c538fbe141c8cbea4d03261d</t>
+  </si>
+  <si>
+    <t>7bed1404c162e3511b71a2ecc62209a929b887701ef218ffc8cec81e04451803</t>
+  </si>
+  <si>
+    <t>2007bca143e865184683cc1c04179df071c45bf7238e2491a310d0a46915311e</t>
+  </si>
+  <si>
+    <t>bebf78f9616a5bbba76513129b493375596cf54f517862ebc4cf94a960e37e7c</t>
+  </si>
+  <si>
+    <t>2b79cff8350c78ab32bb555e62dabdd780560b09fb846acd6cd52edcb37bec8d</t>
+  </si>
+  <si>
+    <t>56e5a229f86e1002bbb6149a63d24e74e92bca855eb390f0d3117cee1d2772f4</t>
+  </si>
+  <si>
+    <t>9572c8e7210fda7fdb8ee8869c8c3b2ff32ebf47331081bfd37ff8b74c2c4ec</t>
+  </si>
+  <si>
+    <t>2f2cccef3d500e530d7fca4daa5009368b0ab6755c3d7ceae2303043ee207ca2</t>
+  </si>
+  <si>
+    <t>fab47aee4c7b22d4f009e7c169d108fa959af51fe2069d200ffc5c1340e6f5bb</t>
+  </si>
+  <si>
+    <t>cfd184a27e9a93e16f790b739def026368ef21085b0bb3e7cbb02e40dc8515df</t>
+  </si>
+  <si>
+    <t>826288bced75b7a118694e0c0b88ad80cb1f921aeb3ab3a3275e6508b5fa4893</t>
+  </si>
+  <si>
+    <t>3a2de610d42831ec0633cdf4a7f9b34c3a75f8de236286c2e6210408f4deda7f</t>
+  </si>
+  <si>
+    <t>0xce560b66d55c71e3ba9d1f671425442e4327777a</t>
+  </si>
+  <si>
+    <t>2edcc1da8c7d489152b72af89c2d331d354d3a6a4f4f6f33081382b8d990c117</t>
+  </si>
+  <si>
+    <t>16e328d22433b30cca921e6201670987165cf1e3783cf85f924eb869f2e0dbc1</t>
+  </si>
+  <si>
+    <t>479c4929a44ab910ce7bb8262997bac29f7691c7e164a372fad03c35919d7651</t>
+  </si>
+  <si>
+    <t>a6bf35446518888e6928bb45cc2d47f186e376ecc41095bd5b98846a2e36a15d</t>
+  </si>
+  <si>
+    <t>c236d50310cbd49f5d3f092e8ec7436a5a0401eac6a786c03045e84e869dba3e</t>
+  </si>
+  <si>
+    <t>0x590821b7cdc36e10f1db94b0e2ba787fc41ae679</t>
+  </si>
+  <si>
+    <t>977a535c9685509bf8db034f022e439c586f84061132c84a1116de1b21643124</t>
+  </si>
+  <si>
+    <t>81d29a450730c15f39bab6cb546b88bfc10dee50f0abf6090f54ccac2ddc7dfd</t>
+  </si>
+  <si>
+    <t>a3ca3689cdeaff70e82e95601636344483ac324391cfcbbf744b557db9bb2860</t>
+  </si>
+  <si>
+    <t>bf1aa1aaeadb60bf901b0622c2de1386c38c1c7564fb64b238762e53ac99b908</t>
+  </si>
+  <si>
+    <t>c6670bc429575348d9c3eb7ab0a9f265ece9880d106530949e5303c09fb7a316</t>
+  </si>
+  <si>
+    <t>0x792f844a1667356271d0c8a8e9cb82a404e52cec</t>
+  </si>
+  <si>
+    <t>996b5597c0a7c59eac562e504ca26736aa3aa489a223e0352a7b8a6e21b5316b</t>
+  </si>
+  <si>
+    <t>ae92130f5e8c83bf926513c71676acfe71602b5d6c9ad52f828be2f07021d51b</t>
+  </si>
+  <si>
+    <t>883dd9dada190b725b181e49f585b40e29674d267c08a91b884db568a0b96816</t>
+  </si>
+  <si>
+    <t>0x4bccc05de8319d6006e74e931d77fb56fd3c339d</t>
+  </si>
+  <si>
+    <t>9d168b649bf1a5afd9f9522b202c910bec62ddaf364b77e6f24bf96eb44d1b5e</t>
+  </si>
+  <si>
+    <t>0x5ac97cb114c413cebea65402fd4484c11a83a0b2</t>
+  </si>
+  <si>
+    <t>fef6be2738cf93deef0fe3884b431084b62c048b20d9f6272bae5d99031909b6</t>
+  </si>
+  <si>
+    <t>c7ea0b62f054569466cd46a3a58095a060eaff4fbe857634c727d5714273bdce</t>
+  </si>
+  <si>
+    <t>3548757c44a5f6e36d072e10aa8d6b602f22783e5a4f05de56028dc4b4507058</t>
+  </si>
+  <si>
+    <t>77d0bce9c03947ffd7d64a4b13981f99a43f35562ff802df2b7e73b916dcdf86</t>
+  </si>
+  <si>
+    <t>0x2667ec978bd182dcc0043d1c1edac934e143a299</t>
+  </si>
+  <si>
+    <t>8cee62671a9e681ebefdab50e3fceb6abaec000e9782527a8dd1836d161d9755</t>
+  </si>
+  <si>
+    <t>b27fa4cae7ccb00627f72536df21385294b5b5f8b19c34dc33c7e6512e4d2564</t>
+  </si>
+  <si>
+    <t>5da9506aeff5fea50adb11136a91b67389b12d92e255f90fe6e31dada75d3f4d</t>
+  </si>
+  <si>
+    <t>0x4148735f1762c3ac174640804c6014a64ea6e98c</t>
+  </si>
+  <si>
+    <t>231f6388656280939ca8ef7c7edb07b903f05c19e08527365f5f4e65f2389ac7</t>
+  </si>
+  <si>
+    <t>0xc79a3d258062d9dac8fddf0cbc4bd3b70bb4278b</t>
+  </si>
+  <si>
+    <t>f3a750e8bfcaf15c2b74b0178a5b538078ac0c8f136bc5e6046926db05d644ee</t>
+  </si>
+  <si>
+    <t>df03d2f546f8227f7724ca83105b0e2c2edce45be35a8c3a20125db3656f09a9</t>
+  </si>
+  <si>
+    <t>1584b80961409bbd47c2a512c2dad65a68de854bd11d5bc52b5bfc67d5df11e5</t>
+  </si>
+  <si>
+    <t>10316c9536f076b5814d346affdbbfc7ed2010f26169d52eea967929710a5ba8</t>
+  </si>
+  <si>
+    <t>0x69d93c0e79cf7c5e07378ef6c5ea8ede5c798d75</t>
+  </si>
+  <si>
+    <t>fd2aac2bd910d352bad5fc2ef6ad30b41ae2c42b03a4617a033ce8e7c6f166fa</t>
+  </si>
+  <si>
+    <t>a2a0daea68dc82abc3f0fe0bd70b43859ba1049454ff602cc85f083892055571</t>
+  </si>
+  <si>
+    <t>e4f92a4114f812dc9e50cee1716981054b0e1ade7da9c04ff568d7677b429ffe</t>
+  </si>
+  <si>
+    <t>0xe87206ee4bc7a2a6e74bcca13ee1a6d16eb4b101</t>
+  </si>
+  <si>
+    <t>abefe620d7b5a042d0bd782232ecba8baf5bc1863e8d614333db9ce2ca7f0e28</t>
+  </si>
+  <si>
+    <t>0x40f49668ae3334d62907da0505b347678bdce712</t>
+  </si>
+  <si>
+    <t>580afca99e4194bc8d4f5ec765985b5317f5258c990459cca4be47d224be3c4</t>
+  </si>
+  <si>
+    <t>ea69a4824902d16d7b4b6e84c851b736ae4fd2b57d789aa11dd1243d4d27b187</t>
+  </si>
+  <si>
+    <t>490d02573d601205f51f7f063e13c4d89d225084c09bf906f63f932668872028</t>
+  </si>
+  <si>
+    <t>45e87769708e46648427114a1637b0de92047a7b4588e2f154458f418470dfa9</t>
+  </si>
+  <si>
+    <t>0x0411a3c75a8813a7537ae06b730ca0076b4c4fd8</t>
+  </si>
+  <si>
+    <t>9d2fe327ad268faebccc2f8a345bbfef1852931daa58e156e32094318a222cc9</t>
+  </si>
+  <si>
+    <t>5b5694f883e6559dffc8b80b3598533ee76f70492e7cabd7ea687bc7fb0d1838</t>
+  </si>
+  <si>
+    <t>a5cf82bc4fdfcc8f74d6489af1b0c7951f6abad1ffce94b37cfa0986bea1a000</t>
+  </si>
+  <si>
+    <t>0x9b13a7afdb5e0156e9ee9325cb372438b5fb9e77</t>
+  </si>
+  <si>
+    <t>a9a4400c19945ac19720c8bfa6d8924a867a324fa1d17b1b7965e55df1c15bf2</t>
+  </si>
+  <si>
+    <t>0x786fce34a45b1c3ac72e73d35b93683da81e8d2a</t>
   </si>
 </sst>
 </file>
@@ -2152,8 +2776,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" hidden="false" style="0" width="70.337890625" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="45.8609375" collapsed="true" outlineLevel="0"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" hidden="false" style="0" width="71.4623046875" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="46.866796875" collapsed="true" outlineLevel="0"/>
     <col min="3" max="5" customWidth="true" hidden="false" style="0" width="44.97" collapsed="true" outlineLevel="0"/>
     <col min="6" max="6" customWidth="true" hidden="false" style="0" width="66.99" collapsed="true" outlineLevel="0"/>
     <col min="7" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
@@ -2178,7 +2802,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>662</v>
+        <v>868</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2186,38 +2810,46 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>663</v>
+        <v>869</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>664</v>
+        <v>870</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>667</v>
+        <v>873</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>669</v>
+        <v>875</v>
       </c>
       <c r="B6" t="s">
-        <v>670</v>
+        <v>876</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>665</v>
+        <v>871</v>
       </c>
       <c r="B7" t="s">
-        <v>666</v>
+        <v>872</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>877</v>
+      </c>
+      <c r="B8" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>668</v>
+        <v>874</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 05 01 2021
</commit_message>
<xml_diff>
--- a/Silamoney/TestData/datafile.xlsx
+++ b/Silamoney/TestData/datafile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="293">
   <si>
     <t xml:space="preserve">privatekeys</t>
   </si>
@@ -818,6 +818,87 @@
   </si>
   <si>
     <t>0x9c62a3519b7c06fbf8d928f300852d23783afb8c</t>
+  </si>
+  <si>
+    <t>75d46f41-a895-4562-9268-506302f1290f</t>
+  </si>
+  <si>
+    <t>59ecb5b2-c194-4366-92af-c8be7a00d602</t>
+  </si>
+  <si>
+    <t>c7d9e1ab3a3c0b59763e7f2c01305f1660950ea7e9ffe3b0ab53f828392bcbd5</t>
+  </si>
+  <si>
+    <t>0x59ea2c576337adc910cda9ef89389b202aeaa2eb</t>
+  </si>
+  <si>
+    <t>c51b2b8a5ad0d8892a4ef06477efe6e2996023e0653555fdabffa3b8e422d616</t>
+  </si>
+  <si>
+    <t>0xcaad62682714605283e2a3eb3afcc3ea6c9be106</t>
+  </si>
+  <si>
+    <t>dbfd618b829cdba9d699e4bff3e041fd00c653d281f730259a1193cf45e256f0</t>
+  </si>
+  <si>
+    <t>0xf4e85a4bf741c23602d4869c3ea4a5e69715866d</t>
+  </si>
+  <si>
+    <t>90aeb9cf322d891e9df6a502988805757a043944d5092ae5ce33f5c5617b2d70</t>
+  </si>
+  <si>
+    <t>0x3e3c5dafc0e10f5d727336fd649e7dde3118963b</t>
+  </si>
+  <si>
+    <t>d216c9081bdd35608241dbe12c42b885a4afd74cb16cdf086bdf377d2ead30dc</t>
+  </si>
+  <si>
+    <t>0x051e13dd01f4b191353deffe82549c7728df456c</t>
+  </si>
+  <si>
+    <t>16be1021d94c01821478936f30168c0e93ba471e5ac6c95d147cc47abf9c1d01</t>
+  </si>
+  <si>
+    <t>0x891cb760f6b14042e75072fd496585366d708b3f</t>
+  </si>
+  <si>
+    <t>2538b44c1b00e95bb61bb72e801a2c8f0555a1985f241add74cce3e02798fc21</t>
+  </si>
+  <si>
+    <t>0x040f726b8e84bd905bb51983386baec823487357</t>
+  </si>
+  <si>
+    <t>55512901600f82c3031a03862bce324939c0b348927bf483a82ce4d738817bd2</t>
+  </si>
+  <si>
+    <t>0xa20cb4aa4710770b2479da9aedc8102c30d9dbcd</t>
+  </si>
+  <si>
+    <t>101c9234913073c96d8a929b3085d2f3a70825de1e208a457e3648bfac109c9e</t>
+  </si>
+  <si>
+    <t>0x5ec2edc0610c3cdcc9bb96d6e47bc69369ebc117</t>
+  </si>
+  <si>
+    <t>60adc85e5bb3d7a265d28fd3cc518317918e8c20cefd1617b94a5b8f35df0dc</t>
+  </si>
+  <si>
+    <t>0x3e6a132c60a81cb71d39ef33d0b9b9d7f2eb56ec</t>
+  </si>
+  <si>
+    <t>dbd2d8b344fe9e223726c19008de8f0aba2e54eb</t>
+  </si>
+  <si>
+    <t>320a70e0ee1c69382041db1dc26617df5645ccbbc00c31b2099209d9341f539b</t>
+  </si>
+  <si>
+    <t>0x9ed59f992b83959ed4fb635cdc09ecee7421e018</t>
+  </si>
+  <si>
+    <t>f100109b-f1d0-4460-bdcf-6a2bdd54940c</t>
+  </si>
+  <si>
+    <t>461e572f-2528-49e6-8741-47692a58a91b</t>
   </si>
 </sst>
 </file>
@@ -940,8 +1021,8 @@
     <col min="1" max="1" bestFit="true" customWidth="true" hidden="false" style="0" width="70.6216796875" collapsed="true" outlineLevel="0"/>
     <col min="2" max="2" bestFit="true" customWidth="true" hidden="false" style="0" width="47.5357421875" collapsed="true" outlineLevel="0"/>
     <col min="3" max="3" customWidth="true" hidden="false" style="0" width="44.97" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" hidden="false" style="0" width="38.5326171875" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" hidden="false" style="0" width="44.091796875" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" hidden="false" style="0" width="38.2955078125" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" hidden="false" style="0" width="43.8609375" collapsed="true" outlineLevel="0"/>
     <col min="6" max="6" customWidth="true" hidden="false" style="0" width="66.99" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
@@ -970,99 +1051,99 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="D2" t="s">
-        <v>250</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="B3" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="D3" t="s">
-        <v>251</v>
+        <v>292</v>
       </c>
       <c r="E3" t="s">
-        <v>247</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="B4" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="B5" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="B7" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>248</v>
+        <v>289</v>
       </c>
       <c r="B8" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="B33" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>243</v>
+        <v>284</v>
       </c>
       <c r="B41" t="s">
-        <v>244</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>241</v>
+        <v>282</v>
       </c>
       <c r="B42" t="s">
-        <v>242</v>
+        <v>283</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>245</v>
+        <v>286</v>
       </c>
       <c r="B51" t="s">
-        <v>246</v>
+        <v>287</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>